<commit_message>
cost precalculated in scenario
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_Building_Action.xlsx
+++ b/projects/test_building/input/ID_Building_Action.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB1215F-9022-EC4F-859F-B01D7E523C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E3363-425C-924A-B830-DE266D017DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5640" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="temp" sheetId="2" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>name</t>
   </si>
@@ -90,6 +91,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C514712E-EDD0-0145-8AB7-7CD7B9C0BA19}" name="Table2" displayName="Table2" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{C514712E-EDD0-0145-8AB7-7CD7B9C0BA19}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{5E1E42B4-6769-E243-90E1-FC8EE9CFF14E}" name="id_building_action"/>
+    <tableColumn id="2" xr3:uid="{33EBF536-D529-E743-98B7-4E9AC256D63B}" name="name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
   <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
@@ -362,11 +374,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6B270B-25A9-0C45-9418-E9C467A5D99F}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="188" workbookViewId="0">
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added the logic of supply temperature influencing the efficiency of heating technologies (only HP) for space heating and hot water separately.
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_Building_Action.xlsx
+++ b/projects/test_building/input/ID_Building_Action.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4E3363-425C-924A-B830-DE266D017DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="765" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="temp" sheetId="2" r:id="rId1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,22 +90,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C514712E-EDD0-0145-8AB7-7CD7B9C0BA19}" name="Table2" displayName="Table2" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3" xr:uid="{C514712E-EDD0-0145-8AB7-7CD7B9C0BA19}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5E1E42B4-6769-E243-90E1-FC8EE9CFF14E}" name="id_building_action"/>
-    <tableColumn id="2" xr3:uid="{33EBF536-D529-E743-98B7-4E9AC256D63B}" name="name"/>
+    <tableColumn id="1" name="id_building_action"/>
+    <tableColumn id="2" name="name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_building_action"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="name"/>
+    <tableColumn id="1" name="id_building_action"/>
+    <tableColumn id="2" name="name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -374,20 +373,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6B270B-25A9-0C45-9418-E9C467A5D99F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -395,7 +394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -403,7 +402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -420,20 +419,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScale="188" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -441,7 +440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -449,7 +448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -457,7 +456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
first draft of scenario-specific input tables.
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_Building_Action.xlsx
+++ b/projects/test_building/input/ID_Building_Action.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="5640" yWindow="765" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="temp" sheetId="2" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="temp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -90,8 +90,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
     <tableColumn id="1" name="id_building_action"/>
     <tableColumn id="2" name="name"/>
@@ -101,8 +101,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
     <tableColumn id="1" name="id_building_action"/>
     <tableColumn id="2" name="name"/>
@@ -374,9 +374,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -416,58 +470,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView zoomScale="188" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
clean-up of input tables
</commit_message>
<xml_diff>
--- a/projects/test_building/input/ID_Building_Action.xlsx
+++ b/projects/test_building/input/ID_Building_Action.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="765" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5640" yWindow="770" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="temp" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>name</t>
   </si>
@@ -92,17 +91,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B4" totalsRowShown="0">
   <autoFilter ref="A1:B4"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="id_building_action"/>
-    <tableColumn id="2" name="name"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3"/>
   <tableColumns count="2">
     <tableColumn id="1" name="id_building_action"/>
     <tableColumn id="2" name="name"/>
@@ -380,13 +368,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -394,7 +382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -402,7 +390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -410,58 +398,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>